<commit_message>
mejoras en el módulo de citas
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistemaClinico\Requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FC94B-41A2-4336-8B6B-8B69782BEAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36732E-9F92-4FC2-878E-9893F4348216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -98,6 +98,39 @@
   <si>
     <t>Reporte 3: Mostrar una agenda de citas para el cliente y una agenda de citas 
 confirmadas para para el odontólogo</t>
+  </si>
+  <si>
+    <t>objetivo 100%</t>
+  </si>
+  <si>
+    <t>gestionar fecha</t>
+  </si>
+  <si>
+    <t>Gestionar Paciente</t>
+  </si>
+  <si>
+    <t>Gestionar Doctor</t>
+  </si>
+  <si>
+    <t>gestionar especialidad</t>
+  </si>
+  <si>
+    <t>historia clínica completa</t>
+  </si>
+  <si>
+    <t>voy a necesitar tiempo para investigar y/o preguntar como funciona todo y los documentos (los datos de la historia clínica, documento para tratamiento, historial tratamiento)</t>
+  </si>
+  <si>
+    <t>Recetas</t>
+  </si>
+  <si>
+    <t>voleta de venta</t>
+  </si>
+  <si>
+    <t>el día miércoles te voy a dar un avance funcionando, le das el visto bueno y sigo agregando más cosas</t>
+  </si>
+  <si>
+    <t>al ver que el sistema será más grande, propongo esto:</t>
   </si>
 </sst>
 </file>
@@ -791,30 +824,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -834,6 +843,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1159,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,34 +1209,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1255,9 +1288,9 @@
       <c r="G6" s="18">
         <v>0.4</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
@@ -1269,12 +1302,12 @@
       <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="32">
         <v>43929</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="18">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1287,12 +1320,12 @@
       <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="30">
         <v>43960</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1313,7 +1346,10 @@
         <v>43963</v>
       </c>
       <c r="G9" s="18">
-        <v>0</v>
+        <v>0.4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,10 +1384,10 @@
       <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="33">
         <v>43966</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="18">
         <v>0</v>
       </c>
@@ -1367,8 +1403,8 @@
       <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="18">
         <v>0</v>
       </c>
@@ -1384,10 +1420,10 @@
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="30">
         <v>43967</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="18">
         <v>0</v>
       </c>
@@ -1403,10 +1439,10 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="30">
         <v>43969</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="18">
         <v>0</v>
       </c>
@@ -1422,10 +1458,10 @@
       <c r="D15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="30">
         <v>43970</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="18">
         <v>0</v>
       </c>
@@ -1439,10 +1475,10 @@
         <v>16</v>
       </c>
       <c r="D16" s="19"/>
-      <c r="E16" s="30">
+      <c r="E16" s="22">
         <v>43971</v>
       </c>
-      <c r="F16" s="31"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1454,55 +1490,97 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="34">
+      <c r="F19" s="24"/>
+      <c r="G19" s="26">
         <f>(SUM(G6:G15)/10)</f>
-        <v>0.04</v>
+        <v>0.26999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="33"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="34"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="33"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="7">
         <v>43957</v>
       </c>
       <c r="F21" s="7">
         <v>43970</v>
       </c>
-      <c r="G21" s="34"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="15"/>
+      <c r="C23" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B3:G3"/>
@@ -1512,6 +1590,11 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E11:F12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se terminó con mostrar la cita con el paciente
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36732E-9F92-4FC2-878E-9893F4348216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC344B-0A77-4CD6-A010-5886CC79EDCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>al ver que el sistema será más grande, propongo esto:</t>
+  </si>
+  <si>
+    <t>Falta Crear cuenta</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1328,10 @@
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="18">
-        <v>1</v>
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1346,7 +1352,7 @@
         <v>43963</v>
       </c>
       <c r="G9" s="18">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
@@ -1499,7 +1505,7 @@
       <c r="F19" s="24"/>
       <c r="G19" s="26">
         <f>(SUM(G6:G15)/10)</f>
-        <v>0.26999999999999996</v>
+        <v>0.27999999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se agregó ĺos archivos de gestionar paciente y algo de avance en el js
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BD7A99-2531-4319-A711-8E8EEE920282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C861832-EE0C-4384-A407-0DC5393F2970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Item</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Diseño, estructura de la base de datos</t>
-  </si>
-  <si>
-    <t>Reporta 2: Mostrar historial de tratamiento</t>
   </si>
   <si>
     <t>Prueba final de desarrollo</t>
@@ -138,13 +135,20 @@
   </si>
   <si>
     <t>gestionar fecha ok</t>
+  </si>
+  <si>
+    <t>Reporta 2: Mostrar historial de tratamiento (esta dentro de historia clínica)
+para el paciente solo es informativo(por cada cita se verá el tratamiento y el detalle del mismo)</t>
+  </si>
+  <si>
+    <t>Falta agregar el campo de estado(confirmar cita)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +349,14 @@
       <i/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -801,8 +813,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,7 +830,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -846,29 +856,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="27" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -891,13 +884,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Énfasis1 2" xfId="1" xr:uid="{FEA80DD9-0443-4ED7-9FD3-43CF49DADD5C}"/>
@@ -1224,406 +1241,390 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="11">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>43957</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43928</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="33">
+        <v>43929</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="31">
+        <v>43960</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>4</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="21">
+        <v>2</v>
+      </c>
+      <c r="D9" s="22">
+        <v>43962</v>
+      </c>
+      <c r="E9" s="22">
+        <v>43963</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>43964</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43965</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
+        <v>43966</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>7</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>8</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1</v>
+      </c>
+      <c r="D13" s="31">
+        <v>43967</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="31">
+        <v>43969</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>10</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="22" t="s">
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="31">
+        <v>43970</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>11</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="23">
+        <v>43971</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="27">
+        <f>(SUM(F6:F15)/10)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="12">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="13">
-        <v>2</v>
-      </c>
-      <c r="E6" s="20">
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="6">
         <v>43957</v>
       </c>
-      <c r="F6" s="6">
-        <v>43928</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
-        <v>2</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25">
-        <v>43929</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="18">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
-        <v>3</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="23">
-        <v>43960</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="12">
-        <v>4</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="38">
-        <v>2</v>
-      </c>
-      <c r="E9" s="39">
-        <v>43962</v>
-      </c>
-      <c r="F9" s="39">
-        <v>43963</v>
-      </c>
-      <c r="G9" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12">
-        <v>5</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="13">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6">
-        <v>43964</v>
-      </c>
-      <c r="F10" s="6">
-        <v>43965</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12">
-        <v>6</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26">
-        <v>43966</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="12">
-        <v>7</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="13">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="12">
-        <v>8</v>
-      </c>
-      <c r="C13" s="21" t="s">
+      <c r="E21" s="6">
+        <v>43970</v>
+      </c>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="23">
-        <v>43967</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="23">
-        <v>43969</v>
-      </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="12">
-        <v>10</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1</v>
-      </c>
-      <c r="E15" s="23">
-        <v>43970</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="12">
-        <v>11</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="30">
-        <v>43971</v>
-      </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="34">
-        <f>(SUM(G6:G15)/10)</f>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="7">
-        <v>43957</v>
-      </c>
-      <c r="F21" s="7">
-        <v>43970</v>
-      </c>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="15" t="s">
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1642,12 +1643,12 @@
   <sheetData>
     <row r="6" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregó el módulo de tratamiento, entre otros avances y correcciones
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C861832-EE0C-4384-A407-0DC5393F2970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2EA116-4218-457B-A3ED-51B7ED25F048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -139,9 +139,6 @@
   <si>
     <t>Reporta 2: Mostrar historial de tratamiento (esta dentro de historia clínica)
 para el paciente solo es informativo(por cada cita se verá el tratamiento y el detalle del mismo)</t>
-  </si>
-  <si>
-    <t>Falta agregar el campo de estado(confirmar cita)</t>
   </si>
 </sst>
 </file>
@@ -863,6 +860,37 @@
     <xf numFmtId="14" fontId="27" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -884,37 +912,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Énfasis1 2" xfId="1" xr:uid="{FEA80DD9-0443-4ED7-9FD3-43CF49DADD5C}"/>
@@ -1241,7 +1238,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,32 +1251,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1326,11 +1323,11 @@
         <v>43928</v>
       </c>
       <c r="F6" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+        <v>0.8</v>
+      </c>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1342,10 +1339,10 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="29">
         <v>43929</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="16">
         <v>1</v>
       </c>
@@ -1360,17 +1357,17 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="27">
         <v>43960</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="16">
         <v>0.7</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="40"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -1422,19 +1419,17 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="30">
         <v>43966</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
@@ -1446,10 +1441,10 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1462,10 +1457,10 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="27">
         <v>43967</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
@@ -1480,10 +1475,10 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="27">
         <v>43969</v>
       </c>
-      <c r="E14" s="32"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="16">
         <v>0</v>
       </c>
@@ -1498,10 +1493,10 @@
       <c r="C15" s="11">
         <v>1</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="27">
         <v>43970</v>
       </c>
-      <c r="E15" s="32"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="16">
         <v>0</v>
       </c>
@@ -1514,47 +1509,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="23">
+      <c r="D16" s="34">
         <v>43971</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="27">
+      <c r="E19" s="36"/>
+      <c r="F19" s="38">
         <f>(SUM(F6:F15)/10)</f>
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="26"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
-      <c r="C21" s="26"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="6">
         <v>43957</v>
       </c>
       <c r="E21" s="6">
         <v>43970</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -1611,6 +1606,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
@@ -1620,11 +1620,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D11:E12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
avance, falta terminar el historial de tratamiento
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2EA116-4218-457B-A3ED-51B7ED25F048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF353522-1C04-4223-BC06-1CD171BE1976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -867,30 +867,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -910,6 +886,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1238,7 +1238,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,32 +1251,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1325,9 +1325,9 @@
       <c r="F6" s="16">
         <v>0.8</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1339,10 +1339,10 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="36">
         <v>43929</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="16">
         <v>1</v>
       </c>
@@ -1357,10 +1357,10 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="34">
         <v>43960</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="16">
         <v>0.7</v>
       </c>
@@ -1419,10 +1419,10 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="37">
         <v>43966</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="16">
         <v>1</v>
       </c>
@@ -1441,10 +1441,10 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="16">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1457,10 +1457,10 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="34">
         <v>43967</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
@@ -1475,10 +1475,10 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="34">
         <v>43969</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="16">
         <v>0</v>
       </c>
@@ -1493,10 +1493,10 @@
       <c r="C15" s="11">
         <v>1</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="34">
         <v>43970</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="16">
         <v>0</v>
       </c>
@@ -1509,47 +1509,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="34">
+      <c r="D16" s="26">
         <v>43971</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="38">
+      <c r="E19" s="28"/>
+      <c r="F19" s="30">
         <f>(SUM(F6:F15)/10)</f>
-        <v>0.57999999999999996</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="37"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="38"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="6">
         <v>43957</v>
       </c>
       <c r="E21" s="6">
         <v>43970</v>
       </c>
-      <c r="F21" s="38"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -1606,11 +1606,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G6:I6"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
@@ -1620,6 +1615,11 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D11:E12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se agregó la lista de los datos personales del paciente en el módulo historia clínica del paciente
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF353522-1C04-4223-BC06-1CD171BE1976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3CBD3F-424D-4075-B902-15F58E300B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -867,6 +867,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -886,30 +910,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1238,7 +1238,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,32 +1251,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1323,11 +1323,11 @@
         <v>43928</v>
       </c>
       <c r="F6" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1339,10 +1339,10 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="29">
         <v>43929</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="16">
         <v>1</v>
       </c>
@@ -1357,10 +1357,10 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="27">
         <v>43960</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="16">
         <v>0.7</v>
       </c>
@@ -1419,10 +1419,10 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="30">
         <v>43966</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="16">
         <v>1</v>
       </c>
@@ -1441,10 +1441,10 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="16">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1457,10 +1457,10 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="27">
         <v>43967</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
@@ -1475,12 +1475,12 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="27">
         <v>43969</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="16">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1493,12 +1493,12 @@
       <c r="C15" s="11">
         <v>1</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="27">
         <v>43970</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,47 +1509,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="26">
+      <c r="D16" s="34">
         <v>43971</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="30">
+      <c r="E19" s="36"/>
+      <c r="F19" s="38">
         <f>(SUM(F6:F15)/10)</f>
-        <v>0.59</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="29"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="30"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
-      <c r="C21" s="29"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="6">
         <v>43957</v>
       </c>
       <c r="E21" s="6">
         <v>43970</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -1606,6 +1606,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
@@ -1615,11 +1620,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D11:E12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se termino con todo el módulo de historia clínica
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3CBD3F-424D-4075-B902-15F58E300B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0993BF-72D6-4D72-9D69-CA96DA27FD4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Item</t>
   </si>
@@ -139,6 +139,9 @@
   <si>
     <t>Reporta 2: Mostrar historial de tratamiento (esta dentro de historia clínica)
 para el paciente solo es informativo(por cada cita se verá el tratamiento y el detalle del mismo)</t>
+  </si>
+  <si>
+    <t>Por ahora no se va a tomar en cuenta</t>
   </si>
 </sst>
 </file>
@@ -810,7 +813,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -867,30 +870,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -911,6 +890,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1237,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,32 +1273,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1323,11 +1345,11 @@
         <v>43928</v>
       </c>
       <c r="F6" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+        <v>0.95</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1339,10 +1361,10 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="36">
         <v>43929</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="16">
         <v>1</v>
       </c>
@@ -1357,10 +1379,10 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="34">
         <v>43960</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="16">
         <v>0.7</v>
       </c>
@@ -1386,28 +1408,34 @@
         <v>43963</v>
       </c>
       <c r="F9" s="16">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="41">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="43">
         <v>2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="44">
         <v>43964</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="44">
         <v>43965</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="45">
         <v>0</v>
       </c>
+      <c r="G10" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -1419,10 +1447,10 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="37">
         <v>43966</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="16">
         <v>1</v>
       </c>
@@ -1441,8 +1469,8 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="16">
         <v>1</v>
       </c>
@@ -1457,10 +1485,10 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="34">
         <v>43967</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
@@ -1475,12 +1503,12 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="34">
         <v>43969</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="16">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1493,12 +1521,12 @@
       <c r="C15" s="11">
         <v>1</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="34">
         <v>43970</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="16">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,47 +1537,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="34">
+      <c r="D16" s="26">
         <v>43971</v>
       </c>
-      <c r="E16" s="35"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="38">
-        <f>(SUM(F6:F15)/10)</f>
-        <v>0.71</v>
+      <c r="E19" s="28"/>
+      <c r="F19" s="30">
+        <f>(SUM(F6,F7,F8,F9,F11,F12,F13,F14,F15)/9)</f>
+        <v>0.8833333333333333</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="37"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="38"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="6">
         <v>43957</v>
       </c>
       <c r="E21" s="6">
         <v>43970</v>
       </c>
-      <c r="F21" s="38"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -1605,12 +1633,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G6:I6"/>
+  <mergeCells count="15">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
@@ -1620,6 +1643,12 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D11:E12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se agregó el registo de cuentas para el inicio de sesión
</commit_message>
<xml_diff>
--- a/Requerimientos/cronograma.xlsx
+++ b/Requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DataMedic\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0993BF-72D6-4D72-9D69-CA96DA27FD4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7037AAD-EE76-498E-8CA5-809DBD10A96B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>al ver que el sistema será más grande, propongo esto:</t>
-  </si>
-  <si>
-    <t>Falta Crear cuenta</t>
   </si>
   <si>
     <t>Módulo para crear usuarios</t>
@@ -362,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,12 +503,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,13 +847,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -870,6 +854,43 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="25" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -891,47 +912,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="27" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="27" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1260,7 +1251,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,32 +1264,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1347,9 +1338,9 @@
       <c r="F6" s="16">
         <v>0.95</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1361,10 +1352,10 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="31">
         <v>43929</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="16">
         <v>1</v>
       </c>
@@ -1379,32 +1370,30 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="29">
         <v>43960</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="46">
         <v>2</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="47">
         <v>43962</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="47">
         <v>43963</v>
       </c>
       <c r="F9" s="16">
@@ -1412,30 +1401,30 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="41">
+      <c r="A10" s="23">
         <v>5</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="25">
         <v>2</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="26">
         <v>43964</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="26">
         <v>43965</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="27">
         <v>0</v>
       </c>
-      <c r="G10" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
+      <c r="G10" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
@@ -1447,30 +1436,30 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="32">
         <v>43966</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="16">
         <v>1</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>7</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="16">
         <v>1</v>
       </c>
@@ -1485,10 +1474,10 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="29">
         <v>43967</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
@@ -1503,10 +1492,10 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="29">
         <v>43969</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="16">
         <v>0.5</v>
       </c>
@@ -1521,10 +1510,10 @@
       <c r="C15" s="11">
         <v>1</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="29">
         <v>43970</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="16">
         <v>0.8</v>
       </c>
@@ -1537,47 +1526,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="26">
+      <c r="D16" s="36">
         <v>43971</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="30">
+      <c r="E19" s="38"/>
+      <c r="F19" s="40">
         <f>(SUM(F6,F7,F8,F9,F11,F12,F13,F14,F15)/9)</f>
-        <v>0.8833333333333333</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
-      <c r="C20" s="29"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="30"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
-      <c r="C21" s="29"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="6">
         <v>43957</v>
       </c>
       <c r="E21" s="6">
         <v>43970</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -1594,12 +1583,12 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -1634,6 +1623,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G10:J10"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
@@ -1643,12 +1638,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D11:E12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1667,12 +1656,12 @@
   <sheetData>
     <row r="6" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>